<commit_message>
worked on getriebe metrics svm excel file
</commit_message>
<xml_diff>
--- a/Maschinelles_Lernen/PythonClassifierApplication_Getriebe/Ergebnisse_SVM_Getriebe.xlsx
+++ b/Maschinelles_Lernen/PythonClassifierApplication_Getriebe/Ergebnisse_SVM_Getriebe.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>TPR</t>
   </si>
@@ -483,7 +483,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C0E8F7E-EB4B-4DDE-903A-0584641624B7}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -882,6 +884,9 @@
       <c r="A25" s="14" t="s">
         <v>7</v>
       </c>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
       <c r="D25" s="12">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
worked on result metrics on motor and getriebe svm
</commit_message>
<xml_diff>
--- a/Maschinelles_Lernen/PythonClassifierApplication_Getriebe/Ergebnisse_SVM_Getriebe.xlsx
+++ b/Maschinelles_Lernen/PythonClassifierApplication_Getriebe/Ergebnisse_SVM_Getriebe.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
   <si>
     <t>TPR</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>(C=1.0)</t>
+  </si>
+  <si>
+    <t>nicht normalisiert</t>
   </si>
 </sst>
 </file>
@@ -481,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C0E8F7E-EB4B-4DDE-903A-0584641624B7}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,6 +539,9 @@
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
       <c r="D3" s="11">
         <v>1000</v>
       </c>
@@ -775,7 +781,7 @@
         <v>0.11867570000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D17" s="12">
         <v>3</v>
       </c>
@@ -796,8 +802,12 @@
         <v>11</v>
       </c>
       <c r="K17" s="18"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="M17" s="18"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D18" s="12">
         <v>4</v>
       </c>
@@ -820,8 +830,14 @@
       <c r="K18" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>9</v>
+      </c>
+      <c r="M18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D19" s="12">
         <v>5</v>
       </c>
@@ -846,24 +862,32 @@
         <f>_xlfn.STDEV.P(E15:E19)</f>
         <v>4.07276952453735E-4</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="2">
+        <f>AVERAGE(G15:G19)</f>
+        <v>7.782886E-2</v>
+      </c>
+      <c r="M19">
+        <f>_xlfn.STDEV.P(G15:G19)</f>
+        <v>1.9257795944499988E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D20" s="12"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D21" s="12"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D22" s="12"/>
     </row>
-    <row r="23" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D23" s="16"/>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
       <c r="H23" s="17"/>
     </row>
-    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="D24" s="6" t="s">
         <v>8</v>
       </c>
@@ -880,7 +904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>7</v>
       </c>
@@ -904,7 +928,10 @@
         <v>7.2771999999999837E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
       <c r="D26" s="12">
         <v>2</v>
       </c>
@@ -922,7 +949,7 @@
         <v>7.5328000000000062E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D27" s="12">
         <v>3</v>
       </c>
@@ -943,8 +970,12 @@
         <v>11</v>
       </c>
       <c r="K27" s="18"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="M27" s="18"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D28" s="12">
         <v>4</v>
       </c>
@@ -967,8 +998,14 @@
       <c r="K28" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" t="s">
+        <v>9</v>
+      </c>
+      <c r="M28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D29" s="12">
         <v>5</v>
       </c>
@@ -993,23 +1030,33 @@
         <f>_xlfn.STDEV.P(E25:E29)</f>
         <v>2.1741493416964876E-4</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" s="2">
+        <f>AVERAGE(G25:G29)</f>
+        <v>1.0591140000000001E-2</v>
+      </c>
+      <c r="M29">
+        <f>_xlfn.STDEV.P(G25:G29)</f>
+        <v>5.9502956766870009E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D30" s="12"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D31" s="12"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D32" s="12"/>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L27:M27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
worked on result evaluation excels of SVM approaches, added several screenshots of SVM results
</commit_message>
<xml_diff>
--- a/Maschinelles_Lernen/PythonClassifierApplication_Getriebe/Ergebnisse_SVM_Getriebe.xlsx
+++ b/Maschinelles_Lernen/PythonClassifierApplication_Getriebe/Ergebnisse_SVM_Getriebe.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="14">
   <si>
     <t>TPR</t>
   </si>
@@ -106,7 +106,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -132,11 +132,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -167,9 +196,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -484,11 +524,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C0E8F7E-EB4B-4DDE-903A-0584641624B7}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -781,7 +819,7 @@
         <v>0.11867570000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D17" s="12">
         <v>3</v>
       </c>
@@ -801,13 +839,21 @@
       <c r="J17" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18" t="s">
+      <c r="K17" s="19"/>
+      <c r="L17" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="M17" s="18"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O17" s="19"/>
+      <c r="P17" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="20"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D18" s="12">
         <v>4</v>
       </c>
@@ -824,20 +870,32 @@
         <f t="shared" si="1"/>
         <v>0.11918689999999998</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K18" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L18" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M18" s="22" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="O18" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="P18" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q18" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D19" s="12">
         <v>5</v>
       </c>
@@ -854,40 +912,56 @@
         <f t="shared" si="1"/>
         <v>0.11924699999999999</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19" s="24">
         <f>AVERAGE(E15:E19)</f>
         <v>0.88072590000000006</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="22">
         <f>_xlfn.STDEV.P(E15:E19)</f>
         <v>4.07276952453735E-4</v>
       </c>
-      <c r="L19" s="2">
+      <c r="L19" s="25">
+        <f>AVERAGE(F15:F19)</f>
+        <v>0.84494884000000003</v>
+      </c>
+      <c r="M19" s="22">
+        <f>_xlfn.STDEV.P(F15:F19)</f>
+        <v>1.7501790692383522E-3</v>
+      </c>
+      <c r="N19" s="25">
         <f>AVERAGE(G15:G19)</f>
         <v>7.782886E-2</v>
       </c>
-      <c r="M19">
+      <c r="O19" s="22">
         <f>_xlfn.STDEV.P(G15:G19)</f>
         <v>1.9257795944499988E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P19" s="25">
+        <f>AVERAGE(H15:H19)</f>
+        <v>0.11927410000000001</v>
+      </c>
+      <c r="Q19" s="23">
+        <f>_xlfn.STDEV.P(H15:H19)</f>
+        <v>4.07276952453735E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D20" s="12"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D21" s="12"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D22" s="12"/>
     </row>
-    <row r="23" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D23" s="16"/>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
       <c r="H23" s="17"/>
     </row>
-    <row r="24" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="D24" s="6" t="s">
         <v>8</v>
       </c>
@@ -904,7 +978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>7</v>
       </c>
@@ -928,7 +1002,7 @@
         <v>7.2771999999999837E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -949,7 +1023,7 @@
         <v>7.5328000000000062E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D27" s="12">
         <v>3</v>
       </c>
@@ -969,13 +1043,21 @@
       <c r="J27" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18" t="s">
+      <c r="K27" s="19"/>
+      <c r="L27" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="M27" s="18"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O27" s="19"/>
+      <c r="P27" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q27" s="20"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D28" s="12">
         <v>4</v>
       </c>
@@ -992,20 +1074,32 @@
         <f t="shared" si="2"/>
         <v>7.3674000000000239E-3</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J28" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="K28" t="s">
+      <c r="K28" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="L28" t="s">
+      <c r="L28" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="M28" t="s">
+      <c r="M28" s="22" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="O28" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="P28" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q28" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D29" s="12">
         <v>5</v>
       </c>
@@ -1022,41 +1116,61 @@
         <f t="shared" si="2"/>
         <v>7.8034999999999632E-3</v>
       </c>
-      <c r="J29" s="2">
+      <c r="J29" s="24">
         <f>AVERAGE(E25:E29)</f>
         <v>0.99244312000000012</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="22">
         <f>_xlfn.STDEV.P(E25:E29)</f>
         <v>2.1741493416964876E-4</v>
       </c>
-      <c r="L29" s="2">
+      <c r="L29" s="25">
+        <f>AVERAGE(F25:F29)</f>
+        <v>0.99506353999999997</v>
+      </c>
+      <c r="M29" s="22">
+        <f>_xlfn.STDEV.P(F25:F29)</f>
+        <v>2.3847099278527425E-4</v>
+      </c>
+      <c r="N29" s="25">
         <f>AVERAGE(G25:G29)</f>
         <v>1.0591140000000001E-2</v>
       </c>
-      <c r="M29">
+      <c r="O29" s="22">
         <f>_xlfn.STDEV.P(G25:G29)</f>
         <v>5.9502956766870009E-4</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P29" s="25">
+        <f>AVERAGE(H25:H29)</f>
+        <v>7.5568799999999881E-3</v>
+      </c>
+      <c r="Q29" s="23">
+        <f>_xlfn.STDEV.P(H25:H29)</f>
+        <v>2.1741493416964873E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D30" s="12"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D31" s="12"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D32" s="12"/>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="P27:Q27"/>
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="J27:K27"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N27:O27"/>
     <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L27:M27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>